<commit_message>
Update latest Excel dashboard (2026-02-10 14:20)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,7 +20,7 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-10 14:13  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-10 14:20  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>0.49</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.38</t>
+    <t>0.48</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.37</t>
   </si>
   <si>
     <t>Health</t>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>219.71</v>
+        <v>221.5</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>-112.4580916030534</v>
+        <v>-114.2480916030534</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>84.48848091603054</v>
+        <v>82.69848091603055</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-10 14:54)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,7 +20,7 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-10 14:49  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-10 14:54  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>221.5</v>
+        <v>222.52</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>-114.2480916030534</v>
+        <v>-115.2680916030534</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>82.69848091603055</v>
+        <v>81.67848091603054</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-11 01:21:36)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-10 14:54  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-11 01:21  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>37 confirmed</t>
+    <t>42 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>13 delivered</t>
+    <t>23 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>0.48</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.37</t>
+    <t>0.76</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.47</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>304.1984809160305</v>
+        <v>350.0000076335878</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>107.2519083969466</v>
+        <v>181.1068702290076</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>222.52</v>
+        <v>238.88</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>-115.2680916030534</v>
+        <v>-57.77312977099237</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>81.67848091603054</v>
+        <v>111.1200076335878</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.5362318840579711</v>
+        <v>0.5675675675675675</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.3513513513513514</v>
+        <v>0.5476190476190477</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-11 13:17:49)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-11 01:21  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-11 13:17  •  FX: 1 USD = 1,602 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>42 confirmed</t>
+    <t>46 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>23 delivered</t>
+    <t>24 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>0.76</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.47</t>
+    <t>0.59</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.21</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>350.0000076335878</v>
+        <v>318.0399563046192</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>181.1068702290076</v>
+        <v>155.5867665418227</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>238.88</v>
+        <v>263.41</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>-57.77312977099237</v>
+        <v>-107.8232334581772</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>111.1200076335878</v>
+        <v>54.62995630461927</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.5675675675675675</v>
+        <v>0.575</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5476190476190477</v>
+        <v>0.5217391304347826</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-11 13:53:07)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,13 +20,13 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-11 13:17  •  FX: 1 USD = 1,602 IQD</t>
+    <t>Generated: 2026-02-11 13:53  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>46 confirmed</t>
+    <t>48 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>0.59</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.21</t>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.51</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>318.0399563046192</v>
+        <v>398.8549694656488</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>155.5867665418227</v>
+        <v>190.2671755725191</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>263.41</v>
+        <v>264.26</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>-107.8232334581772</v>
+        <v>-73.99282442748091</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>54.62995630461927</v>
+        <v>134.5949694656488</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.575</v>
+        <v>0.5925925925925926</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5217391304347826</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-11 15:18:50)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,13 +20,13 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-11 14:07  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-11 15:18  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>48 confirmed</t>
+    <t>50 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>0.72</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.51</t>
+    <t>0.71</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.57</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,7 +637,7 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>398.8549694656488</v>
+        <v>418.7022977099236</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>264.26</v>
+        <v>266.87</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>-73.99282442748091</v>
+        <v>-76.60282442748093</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>134.5949694656488</v>
+        <v>151.8322977099236</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.5925925925925926</v>
+        <v>0.5813953488372093</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-11 17:35:09)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-11 15:18  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-11 17:35  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>50 confirmed</t>
+    <t>52 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>24 delivered</t>
+    <t>26 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>0.71</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.57</t>
+    <t>0.81</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.72</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>418.7022977099236</v>
+        <v>438.9313053435114</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>190.2671755725191</v>
+        <v>205.9160305343511</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>266.87</v>
+        <v>254.89</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>-76.60282442748093</v>
+        <v>-48.97396946564885</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>151.8322977099236</v>
+        <v>184.0413053435114</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.5813953488372093</v>
+        <v>0.5909090909090909</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.48</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-12 00:12:15)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,7 +20,7 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-11 17:35  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-12 00:12  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
@@ -32,7 +32,7 @@
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>26 delivered</t>
+    <t>29 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>0.81</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.72</t>
+    <t>0.84</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.56</t>
   </si>
   <si>
     <t>Health</t>
@@ -642,7 +642,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>205.9160305343511</v>
+        <v>236.8320610687023</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>254.89</v>
+        <v>281.88</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>-48.97396946564885</v>
+        <v>-45.04793893129769</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>184.0413053435114</v>
+        <v>157.0513053435114</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5</v>
+        <v>0.5576923076923077</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-12 10:22:39)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,7 +20,7 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-12 00:12  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-12 10:22  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
@@ -32,7 +32,7 @@
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>29 delivered</t>
+    <t>31 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>0.84</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.56</t>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.53</t>
   </si>
   <si>
     <t>Health</t>
@@ -642,7 +642,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>236.8320610687023</v>
+        <v>255.9160305343511</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>281.88</v>
+        <v>287.51</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>-45.04793893129769</v>
+        <v>-31.59396946564885</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>157.0513053435114</v>
+        <v>151.4213053435114</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.5909090909090909</v>
+        <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5576923076923077</v>
+        <v>0.5961538461538461</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-12 17:49:38)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-12 10:22  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-12 17:49  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>52 confirmed</t>
+    <t>58 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>31 delivered</t>
+    <t>33 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>0.89</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.53</t>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.63</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>438.9313053435114</v>
+        <v>487.4045877862595</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>255.9160305343511</v>
+        <v>275.763358778626</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>287.51</v>
+        <v>299.79</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>-31.59396946564885</v>
+        <v>-24.02664122137406</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>151.4213053435114</v>
+        <v>187.6145877862595</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.5714285714285714</v>
+        <v>0.6041666666666666</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5961538461538461</v>
+        <v>0.5689655172413793</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-12 23:05:34)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,7 +20,7 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-12 17:49  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-12 23:05  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
@@ -32,7 +32,7 @@
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>33 delivered</t>
+    <t>35 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>0.92</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.63</t>
+    <t>0.93</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.59</t>
   </si>
   <si>
     <t>Health</t>
@@ -642,7 +642,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>275.763358778626</v>
+        <v>285.6870229007633</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>299.79</v>
+        <v>306.28</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>-24.02664122137406</v>
+        <v>-20.59297709923663</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>187.6145877862595</v>
+        <v>181.1245877862596</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5689655172413793</v>
+        <v>0.603448275862069</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-13 19:55:15)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-12 23:05  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-13 19:55  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>58 confirmed</t>
+    <t>66 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>35 delivered</t>
+    <t>40 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>0.93</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.59</t>
+    <t>1.03</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.73</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>487.4045877862595</v>
+        <v>563.740465648855</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>285.6870229007633</v>
+        <v>336.0687022900763</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>306.28</v>
+        <v>326.51</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>-20.59297709923663</v>
+        <v>9.558702290076326</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>181.1245877862596</v>
+        <v>237.230465648855</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6041666666666666</v>
+        <v>0.6285714285714286</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.603448275862069</v>
+        <v>0.6060606060606061</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -789,7 +789,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5">
-        <v>0</v>
+        <v>30.91603053435114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-14 01:29:06)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,13 +20,13 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-13 19:58  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-14 01:29  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>66 confirmed</t>
+    <t>68 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.03</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.73</t>
+    <t>1.01</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.75</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>563.740465648855</v>
+        <v>583.5877938931297</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>336.0687022900763</v>
+        <v>336.0687022900764</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>326.51</v>
+        <v>333.56</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>9.558702290076326</v>
+        <v>2.508702290076371</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>237.230465648855</v>
+        <v>250.0277938931297</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6285714285714286</v>
+        <v>0.6415094339622641</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.6060606060606061</v>
+        <v>0.5882352941176471</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-14 18:37:19)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-14 01:29  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-14 18:37  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>68 confirmed</t>
+    <t>76 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>40 delivered</t>
+    <t>41 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.01</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.75</t>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.81</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>583.5877938931297</v>
+        <v>654.5801603053434</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>336.0687022900764</v>
+        <v>345.9923664122138</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>333.56</v>
+        <v>362.3499999999999</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>2.508702290076371</v>
+        <v>-16.35763358778615</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>250.0277938931297</v>
+        <v>292.2301603053435</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6415094339622641</v>
+        <v>0.6333333333333333</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5882352941176471</v>
+        <v>0.5394736842105263</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-15 00:04:44)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-14 18:37  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-15 00:04  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>76 confirmed</t>
+    <t>77 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>41 delivered</t>
+    <t>44 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>0.95</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.81</t>
+    <t>9.19</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 16.24</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>654.5801603053434</v>
+        <v>664.8855038167939</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>345.9923664122138</v>
+        <v>376.145038167939</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>362.3499999999999</v>
+        <v>40.94</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>-16.35763358778615</v>
+        <v>335.205038167939</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>292.2301603053435</v>
+        <v>623.9455038167939</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6333333333333333</v>
+        <v>0.6311475409836066</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5394736842105263</v>
+        <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-15 00:05:42)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,7 +20,7 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-15 00:04  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-15 00:05  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>9.19</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 16.24</t>
+    <t>1.01</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.79</t>
   </si>
   <si>
     <t>Health</t>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>40.94</v>
+        <v>371.41</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>335.205038167939</v>
+        <v>4.735038167939024</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>623.9455038167939</v>
+        <v>293.4755038167939</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-15 12:09:31)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-15 00:05  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-15 12:09  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>77 confirmed</t>
+    <t>86 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>44 delivered</t>
+    <t>45 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.01</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.79</t>
+    <t>0.99</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.93</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>664.8855038167939</v>
+        <v>757.2519160305344</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>376.145038167939</v>
+        <v>386.4503816793894</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>371.41</v>
+        <v>391.98</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>4.735038167939024</v>
+        <v>-5.529618320610666</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>293.4755038167939</v>
+        <v>365.2719160305344</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6311475409836066</v>
+        <v>0.6417910447761194</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5714285714285714</v>
+        <v>0.5232558139534884</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-15 13:19:13)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-15 12:09  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-15 13:19  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>86 confirmed</t>
+    <t>87 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>45 delivered</t>
+    <t>46 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>0.99</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.93</t>
+    <t>1.01</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.95</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>757.2519160305344</v>
+        <v>767.1755801526717</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>386.4503816793894</v>
+        <v>396.3740458015267</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>391.98</v>
+        <v>394.33</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>-5.529618320610666</v>
+        <v>2.044045801526693</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>365.2719160305344</v>
+        <v>372.8455801526717</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6417910447761194</v>
+        <v>0.6492537313432836</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5232558139534884</v>
+        <v>0.5287356321839081</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-15 17:58:33)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-15 13:19  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-15 17:58  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>87 confirmed</t>
+    <t>89 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>46 delivered</t>
+    <t>53 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.01</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.95</t>
+    <t>1.13</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.96</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>767.1755801526717</v>
+        <v>786.2595496183205</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>396.3740458015267</v>
+        <v>453.6259541984733</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>394.33</v>
+        <v>401.46</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>2.044045801526693</v>
+        <v>52.16595419847329</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>372.8455801526717</v>
+        <v>384.7995496183205</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6492537313432836</v>
+        <v>0.6267605633802817</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5287356321839081</v>
+        <v>0.5955056179775281</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-15 22:13:30)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,13 +20,13 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-15 17:58  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-15 22:13  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>89 confirmed</t>
+    <t>92 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
@@ -56,7 +56,7 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.13</t>
+    <t>1.10</t>
   </si>
   <si>
     <t>Potential ROAS: 1.96</t>
@@ -637,7 +637,7 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>786.2595496183205</v>
+        <v>808.7786335877863</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>401.46</v>
+        <v>411.96</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>52.16595419847329</v>
+        <v>41.66595419847329</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>384.7995496183205</v>
+        <v>396.8186335877863</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6267605633802817</v>
+        <v>0.6388888888888888</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5955056179775281</v>
+        <v>0.5760869565217391</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-16 10:57:17)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,13 +20,13 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-15 22:57  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-16 10:57  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>92 confirmed</t>
+    <t>96 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.10</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.96</t>
+    <t>1.17</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 2.17</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,7 +637,7 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>808.7786335877863</v>
+        <v>842.7480992366412</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>411.96</v>
+        <v>388.4</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>41.66595419847329</v>
+        <v>65.22595419847335</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>396.8186335877863</v>
+        <v>454.3480992366412</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6388888888888888</v>
+        <v>0.6620689655172414</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5760869565217391</v>
+        <v>0.5520833333333334</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -789,7 +789,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5">
-        <v>30.91603053435114</v>
+        <v>85.87786259541984</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-16 14:33:34)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-16 10:57  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-16 14:33  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>96 confirmed</t>
+    <t>98 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>53 delivered</t>
+    <t>55 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.17</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 2.17</t>
+    <t>1.07</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.95</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>842.7480992366412</v>
+        <v>862.213748091603</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>453.6259541984733</v>
+        <v>472.3282442748092</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>388.4</v>
+        <v>441.75</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>65.22595419847335</v>
+        <v>30.57824427480915</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>454.3480992366412</v>
+        <v>420.463748091603</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6620689655172414</v>
+        <v>0.6712328767123288</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5520833333333334</v>
+        <v>0.5612244897959183</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-17 12:59:04)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-16 14:33  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-17 12:59  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>98 confirmed</t>
+    <t>102 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>55 delivered</t>
+    <t>62 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.07</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.95</t>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.85</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>862.213748091603</v>
+        <v>903.0534427480915</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>472.3282442748092</v>
+        <v>540.2671755725189</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>441.75</v>
+        <v>487.15</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>30.57824427480915</v>
+        <v>53.11717557251887</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>420.463748091603</v>
+        <v>415.9034427480914</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6712328767123288</v>
+        <v>0.6455696202531646</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.5612244897959183</v>
+        <v>0.6078431372549019</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -789,7 +789,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5">
-        <v>85.87786259541984</v>
+        <v>158.587786259542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-17 21:00:19)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-17 12:59  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-17 21:00  •  FX: 1 USD = 1,610 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>102 confirmed</t>
+    <t>107 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>62 delivered</t>
+    <t>69 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.11</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.85</t>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.52</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>903.0534427480915</v>
+        <v>775.7764037267081</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>540.2671755725189</v>
+        <v>496.1180124223603</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>487.15</v>
+        <v>509.2</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>53.11717557251887</v>
+        <v>-13.08198757763978</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>415.9034427480914</v>
+        <v>266.576403726708</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6455696202531646</v>
+        <v>0.6604938271604939</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.6078431372549019</v>
+        <v>0.6448598130841121</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -789,7 +789,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5">
-        <v>158.587786259542</v>
+        <v>129.0372670807454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-17 21:45:38)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,7 +20,7 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-17 21:00  •  FX: 1 USD = 1,610 IQD</t>
+    <t>Generated: 2026-02-17 21:45  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>0.97</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.52</t>
+    <t>1.20</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.87</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>775.7764037267081</v>
+        <v>953.4351221374044</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>496.1180124223603</v>
+        <v>609.7328244274809</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -686,7 +686,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>-13.08198757763978</v>
+        <v>100.5328244274808</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>266.576403726708</v>
+        <v>444.2351221374043</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -789,7 +789,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5">
-        <v>129.0372670807454</v>
+        <v>158.587786259542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-17 23:43:58)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,7 +20,7 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-17 21:45  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-17 23:43  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
@@ -32,7 +32,7 @@
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>69 delivered</t>
+    <t>71 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -59,7 +59,7 @@
     <t>1.20</t>
   </si>
   <si>
-    <t>Potential ROAS: 1.87</t>
+    <t>Potential ROAS: 1.83</t>
   </si>
   <si>
     <t>Health</t>
@@ -642,7 +642,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>609.7328244274809</v>
+        <v>621.5648854961831</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>509.2</v>
+        <v>520.0599999999999</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>100.5328244274808</v>
+        <v>101.5048854961832</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>444.2351221374043</v>
+        <v>433.3751221374044</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.6448598130841121</v>
+        <v>0.6635514018691588</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-18 12:38:33)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,13 +20,13 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-18 00:14  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-18 12:38  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>107 confirmed</t>
+    <t>109 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.20</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.83</t>
+    <t>1.16</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.82</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,7 +637,7 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>953.4351221374044</v>
+        <v>977.0992442748091</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>520.0599999999999</v>
+        <v>535.83</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>101.5048854961832</v>
+        <v>85.7348854961831</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>433.3751221374044</v>
+        <v>441.269244274809</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6604938271604939</v>
+        <v>0.6449704142011834</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.6635514018691588</v>
+        <v>0.6513761467889908</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -789,7 +789,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5">
-        <v>158.587786259542</v>
+        <v>221.1832061068702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-18 23:48:38)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-18 12:38  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-18 23:48  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>109 confirmed</t>
+    <t>112 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>71 delivered</t>
+    <t>72 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.16</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.82</t>
+    <t>1.15</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.84</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>977.0992442748091</v>
+        <v>1012.213748091603</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>621.5648854961831</v>
+        <v>631.8702290076335</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>535.83</v>
+        <v>549.29</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>85.7348854961831</v>
+        <v>82.58022900763353</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>441.269244274809</v>
+        <v>462.923748091603</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6449704142011834</v>
+        <v>0.6511627906976745</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.6513761467889908</v>
+        <v>0.6428571428571429</v>
       </c>
     </row>
     <row r="23" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-20 01:50:15)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-18 23:48  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-20 01:50  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>112 confirmed</t>
+    <t>117 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>72 delivered</t>
+    <t>74 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.15</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.84</t>
+    <t>1.07</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.76</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>1012.213748091603</v>
+        <v>1063.740465648855</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>631.8702290076335</v>
+        <v>643.7022900763358</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>549.29</v>
+        <v>603.53</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>82.58022900763353</v>
+        <v>40.1722900763358</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>462.923748091603</v>
+        <v>460.210465648855</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6511627906976745</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.6428571428571429</v>
+        <v>0.6324786324786325</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -781,7 +781,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="8">
-        <v>0</v>
+        <v>0.01351351351351351</v>
       </c>
     </row>
     <row r="24" spans="2:8">
@@ -789,7 +789,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5">
-        <v>221.1832061068702</v>
+        <v>346.3740458015267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-20 12:47:45)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-20 01:50  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-20 12:47  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>117 confirmed</t>
+    <t>128 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>74 delivered</t>
+    <t>76 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.07</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.76</t>
+    <t>1.06</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.92</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>1063.740465648855</v>
+        <v>1201.908404580153</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>643.7022900763358</v>
+        <v>663.5496183206105</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>603.53</v>
+        <v>624.6</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>40.1722900763358</v>
+        <v>38.94961832061051</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>460.210465648855</v>
+        <v>577.3084045801528</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.65</v>
+        <v>0.6464646464646465</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.6324786324786325</v>
+        <v>0.59375</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -781,7 +781,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="8">
-        <v>0.01351351351351351</v>
+        <v>0.0131578947368421</v>
       </c>
     </row>
     <row r="24" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-20 23:17:03)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-20 12:47  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-20 23:17  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>128 confirmed</t>
+    <t>135 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>76 delivered</t>
+    <t>83 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.06</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.92</t>
+    <t>1.17</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 2.01</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>1201.908404580153</v>
+        <v>1279.007641221374</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>663.5496183206105</v>
+        <v>744.4656488549617</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>624.6</v>
+        <v>634.78</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>38.94961832061051</v>
+        <v>109.6856488549618</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>577.3084045801528</v>
+        <v>644.2276412213739</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6464646464646465</v>
+        <v>0.6553398058252428</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.59375</v>
+        <v>0.6148148148148148</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -781,7 +781,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="8">
-        <v>0.0131578947368421</v>
+        <v>0.01204819277108434</v>
       </c>
     </row>
     <row r="24" spans="2:8">

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-21 21:38:18)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-20 23:17  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-21 21:38  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>135 confirmed</t>
+    <t>138 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>83 delivered</t>
+    <t>93 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.17</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 2.01</t>
+    <t>1.33</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 2.02</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>1279.007641221374</v>
+        <v>1317.175580152672</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>744.4656488549617</v>
+        <v>871.564885496183</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>634.78</v>
+        <v>652.96</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>109.6856488549618</v>
+        <v>218.604885496183</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>644.2276412213739</v>
+        <v>664.2155801526717</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6553398058252428</v>
+        <v>0.6509433962264151</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.6148148148148148</v>
+        <v>0.6739130434782609</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -781,7 +781,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="8">
-        <v>0.01204819277108434</v>
+        <v>0.01075268817204301</v>
       </c>
     </row>
     <row r="24" spans="2:8">
@@ -789,7 +789,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5">
-        <v>346.3740458015267</v>
+        <v>402.8625954198474</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-21 22:54:09)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,7 +20,7 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-21 21:38  •  FX: 1 USD = 1,310 IQD</t>
+    <t>Generated: 2026-02-21 22:54  •  FX: 1 USD = 1,600 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.33</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 2.02</t>
+    <t>1.09</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 1.65</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>1317.175580152672</v>
+        <v>1078.43750625</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>871.564885496183</v>
+        <v>713.59375</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -686,7 +686,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>218.604885496183</v>
+        <v>60.63374999999996</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>664.2155801526717</v>
+        <v>425.47750625</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -789,7 +789,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5">
-        <v>402.8625954198474</v>
+        <v>329.84375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update latest Excel dashboard (2026-02-22 18:08:09)
</commit_message>
<xml_diff>
--- a/data/latest_dashboard.xlsx
+++ b/data/latest_dashboard.xlsx
@@ -20,19 +20,19 @@
     <t>E-commerce Dashboard</t>
   </si>
   <si>
-    <t>Generated: 2026-02-21 22:54  •  FX: 1 USD = 1,600 IQD</t>
+    <t>Generated: 2026-02-22 18:08  •  FX: 1 USD = 1,310 IQD</t>
   </si>
   <si>
     <t>Confirmed Profit (USD)</t>
   </si>
   <si>
-    <t>138 confirmed</t>
+    <t>144 confirmed</t>
   </si>
   <si>
     <t>Delivered Profit (USD)</t>
   </si>
   <si>
-    <t>93 delivered</t>
+    <t>99 delivered</t>
   </si>
   <si>
     <t>Ad Spend (USD)</t>
@@ -56,10 +56,10 @@
     <t>ROAS (Realized)</t>
   </si>
   <si>
-    <t>1.09</t>
-  </si>
-  <si>
-    <t>Potential ROAS: 1.65</t>
+    <t>1.41</t>
+  </si>
+  <si>
+    <t>Potential ROAS: 2.06</t>
   </si>
   <si>
     <t>Health</t>
@@ -637,12 +637,12 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="5">
-        <v>1078.43750625</v>
+        <v>1383.206114503817</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="5">
-        <v>713.59375</v>
+        <v>948.6641221374045</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -681,12 +681,12 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="5">
-        <v>652.96</v>
+        <v>672.1199999999999</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="F11" s="5">
-        <v>60.63374999999996</v>
+        <v>276.5441221374047</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="5">
-        <v>425.47750625</v>
+        <v>711.0861145038168</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="8">
-        <v>0.6509433962264151</v>
+        <v>0.631578947368421</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -773,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="8">
-        <v>0.6739130434782609</v>
+        <v>0.6875</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -781,7 +781,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="8">
-        <v>0.01075268817204301</v>
+        <v>0.0101010101010101</v>
       </c>
     </row>
     <row r="24" spans="2:8">
@@ -789,7 +789,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5">
-        <v>329.84375</v>
+        <v>444.4656488549618</v>
       </c>
     </row>
   </sheetData>

</xml_diff>